<commit_message>
Marks UnitDailyEnergy approved if there is nothing to approve (no energy positions)
</commit_message>
<xml_diff>
--- a/Documentation/Месечна Форма..xlsx
+++ b/Documentation/Месечна Форма..xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="240" yWindow="45" windowWidth="18195" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Въглеводороди" sheetId="1" r:id="rId1"/>
+    <sheet name="Свежа Вода" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Въглеводороди!$B$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="63">
   <si>
     <t>Код</t>
   </si>
@@ -185,13 +186,34 @@
   </si>
   <si>
     <t>Редакция</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + Производство АВД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Инсталация АД 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Консумирана Свежа Вода</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Произведено</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Химикали</t>
+  </si>
+  <si>
+    <t>Инсталация</t>
+  </si>
+  <si>
+    <t>Оперативни данни</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,15 +232,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -281,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -405,54 +418,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -761,11 +803,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,569 +824,1272 @@
     <col min="10" max="10" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2">
         <v>6838.68</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F5" s="2">
         <v>6838.68</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
         <v>115.89</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F6" s="2">
         <v>115.89</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
         <v>6954.57</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F8" s="2">
         <v>6954.57</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
         <v>26.16</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F10" s="2">
         <v>26.16</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="16"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2">
+        <v>74.3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>74.3</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2">
+        <v>373.38</v>
+      </c>
+      <c r="F13" s="2">
+        <v>373.38</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2">
+        <v>650.96</v>
+      </c>
+      <c r="F14" s="2">
+        <v>650.96</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2">
+        <v>641.07000000000005</v>
+      </c>
+      <c r="F15" s="2">
+        <v>641.07000000000005</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>693.9</v>
+      </c>
+      <c r="F16" s="2">
+        <v>693.9</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2">
+        <v>839.47</v>
+      </c>
+      <c r="F17" s="2">
+        <v>839.47</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3661.28</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3661.28</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2">
+        <v>6960.52</v>
+      </c>
+      <c r="F21" s="2">
+        <v>6960.52</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2">
+        <v>13.9</v>
+      </c>
+      <c r="F22" s="2">
+        <v>13.9</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2">
+        <v>6974.42</v>
+      </c>
+      <c r="F23" s="2">
+        <v>6974.42</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="2">
+        <v>23.64</v>
+      </c>
+      <c r="F25" s="2">
+        <v>23.64</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="F26" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="2">
+        <v>216.28</v>
+      </c>
+      <c r="F27" s="2">
+        <v>216.28</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="2">
+        <v>24.34</v>
+      </c>
+      <c r="F28" s="2">
+        <v>24.34</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A24:J24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="21"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6838.68</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6838.68</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2">
+        <v>115.89</v>
+      </c>
+      <c r="G5" s="2">
+        <v>115.89</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6954.57</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6954.57</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2">
+        <v>26.16</v>
+      </c>
+      <c r="G9" s="2">
+        <v>26.16</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2">
         <v>74.3</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G11" s="2">
         <v>74.3</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
+      <c r="H11" s="2"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2">
         <v>373.38</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G12" s="2">
         <v>373.38</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
+      <c r="H12" s="2"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2">
         <v>650.96</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G13" s="2">
         <v>650.96</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
+      <c r="H13" s="2"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="2">
         <v>641.07000000000005</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G14" s="2">
         <v>641.07000000000005</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="15"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
+      <c r="H14" s="2"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2">
         <v>693.9</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G15" s="2">
         <v>693.9</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+      <c r="H15" s="2"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2">
         <v>839.47</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G16" s="2">
         <v>839.47</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="H16" s="2"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2">
         <v>0</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G17" s="2">
         <v>0</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="4">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="2">
         <v>0</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G18" s="2">
         <v>0</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="4">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="2">
         <v>3661.28</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G19" s="2">
         <v>3661.28</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
+      <c r="H19" s="2"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="4">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="2">
         <v>6960.52</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G20" s="2">
         <v>6960.52</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
+      <c r="H20" s="2"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="2">
         <v>13.9</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G21" s="2">
         <v>13.9</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="4">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2">
         <v>6974.42</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G22" s="2">
         <v>6974.42</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="16"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
+      <c r="H22" s="2"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="4">
+      <c r="F24" s="2">
         <v>23.64</v>
       </c>
-      <c r="F23" s="4">
+      <c r="G24" s="2">
         <v>23.64</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4" t="s">
+      <c r="H24" s="2"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="4">
+      <c r="F25" s="2">
         <v>15.99</v>
       </c>
-      <c r="F24" s="4">
+      <c r="G25" s="2">
         <v>15.99</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
+      <c r="H25" s="2"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="4">
+      <c r="F26" s="2">
         <v>216.28</v>
       </c>
-      <c r="F25" s="4">
+      <c r="G26" s="2">
         <v>216.28</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4" t="s">
+      <c r="H26" s="2"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="4">
+      <c r="F27" s="2">
         <v>24.34</v>
       </c>
-      <c r="F26" s="4">
+      <c r="G27" s="2">
         <v>24.34</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="15"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A7:J7"/>
+  <mergeCells count="5">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>